<commit_message>
Atualização automática do relatório BI
</commit_message>
<xml_diff>
--- a/Relatório Construção.xlsx
+++ b/Relatório Construção.xlsx
@@ -847,7 +847,7 @@
         <v>45817.43766342592</v>
       </c>
       <c r="AW2">
-        <v>146.814201</v>
+        <v>146.855856</v>
       </c>
     </row>
     <row r="3" ht="18" customHeight="1">
@@ -948,7 +948,7 @@
         <v>45951.64880045139</v>
       </c>
       <c r="AK3">
-        <v>12.603067</v>
+        <v>12.644722</v>
       </c>
     </row>
     <row r="4" ht="18" customHeight="1">
@@ -1052,7 +1052,7 @@
         <v>45926.59935224536</v>
       </c>
       <c r="AK4">
-        <v>37.652512</v>
+        <v>37.694167</v>
       </c>
     </row>
     <row r="5" ht="18" customHeight="1">
@@ -1191,7 +1191,7 @@
         <v>45954.64831328703</v>
       </c>
       <c r="AQ5">
-        <v>9.603553</v>
+        <v>9.645208</v>
       </c>
     </row>
     <row r="6" ht="18" customHeight="1">
@@ -1367,7 +1367,7 @@
         <v>45862.49200517361</v>
       </c>
       <c r="AW6">
-        <v>101.759861</v>
+        <v>101.801516</v>
       </c>
     </row>
     <row r="7" ht="18" customHeight="1">
@@ -1545,7 +1545,7 @@
         <v>45859.70545487269</v>
       </c>
       <c r="AW7">
-        <v>104.546412</v>
+        <v>104.588067</v>
       </c>
     </row>
     <row r="8" ht="18" customHeight="1">
@@ -1646,7 +1646,7 @@
         <v>45959.60034671296</v>
       </c>
       <c r="AK8">
-        <v>4.651528</v>
+        <v>4.693183</v>
       </c>
     </row>
     <row r="9" ht="18" customHeight="1">
@@ -1824,7 +1824,7 @@
         <v>45824.66795922453</v>
       </c>
       <c r="AW9">
-        <v>139.583912</v>
+        <v>139.625567</v>
       </c>
     </row>
     <row r="10" ht="18" customHeight="1">
@@ -2008,7 +2008,7 @@
         <v>45875.62732515046</v>
       </c>
       <c r="AW10">
-        <v>88.624549</v>
+        <v>88.66620399999999</v>
       </c>
     </row>
     <row r="11" ht="18" customHeight="1">
@@ -2189,7 +2189,7 @@
         <v>45890.64166144676</v>
       </c>
       <c r="AW11">
-        <v>73.610208</v>
+        <v>73.65186300000001</v>
       </c>
     </row>
     <row r="12" ht="18" customHeight="1">
@@ -2367,7 +2367,7 @@
         <v>45891.54403121528</v>
       </c>
       <c r="AW12">
-        <v>72.707836</v>
+        <v>72.74949100000001</v>
       </c>
     </row>
     <row r="13" ht="18" customHeight="1">
@@ -2477,7 +2477,7 @@
         <v>45947.74549739584</v>
       </c>
       <c r="AN13">
-        <v>16.506377</v>
+        <v>16.548032</v>
       </c>
     </row>
     <row r="14" ht="18" customHeight="1">
@@ -2655,7 +2655,7 @@
         <v>45812.58396733797</v>
       </c>
       <c r="AW14">
-        <v>151.667905</v>
+        <v>151.70956</v>
       </c>
     </row>
     <row r="15" ht="18" customHeight="1">
@@ -2833,7 +2833,7 @@
         <v>45826.76881550926</v>
       </c>
       <c r="AW15">
-        <v>137.483056</v>
+        <v>137.524711</v>
       </c>
     </row>
     <row r="16" ht="18" customHeight="1">
@@ -3011,7 +3011,7 @@
         <v>45856.44733234953</v>
       </c>
       <c r="AW16">
-        <v>106.611586</v>
+        <v>106.653241</v>
       </c>
     </row>
     <row r="17" ht="18" customHeight="1">
@@ -3192,7 +3192,7 @@
         <v>45855.34298560185</v>
       </c>
       <c r="AW17">
-        <v>108.908889</v>
+        <v>108.950544</v>
       </c>
     </row>
     <row r="18" ht="18" customHeight="1">
@@ -3335,7 +3335,7 @@
         <v>45939.61831496528</v>
       </c>
       <c r="AN18">
-        <v>11.781921</v>
+        <v>11.823576</v>
       </c>
       <c r="AO18" s="2">
         <v>45939.61831515047</v>
@@ -3457,7 +3457,7 @@
         <v>45952.60955998843</v>
       </c>
       <c r="AN19">
-        <v>11.642315</v>
+        <v>11.68397</v>
       </c>
     </row>
     <row r="20" ht="18" customHeight="1">
@@ -3638,7 +3638,7 @@
         <v>45887.7561505787</v>
       </c>
       <c r="AW20">
-        <v>76.495718</v>
+        <v>76.537373</v>
       </c>
     </row>
     <row r="21" ht="18" customHeight="1">
@@ -3819,7 +3819,7 @@
         <v>45895.66738841435</v>
       </c>
       <c r="AW21">
-        <v>68.584479</v>
+        <v>68.62613399999999</v>
       </c>
     </row>
     <row r="22" ht="18" customHeight="1">
@@ -3923,7 +3923,7 @@
         <v>45908.53439914352</v>
       </c>
       <c r="AK22">
-        <v>55.717465</v>
+        <v>55.75912</v>
       </c>
     </row>
     <row r="23" ht="18" customHeight="1">
@@ -4024,7 +4024,7 @@
         <v>45959.6003316088</v>
       </c>
       <c r="AK23">
-        <v>4.651539</v>
+        <v>4.693194</v>
       </c>
     </row>
     <row r="24" ht="18" customHeight="1">
@@ -4125,7 +4125,7 @@
         <v>45959.60028087963</v>
       </c>
       <c r="AK24">
-        <v>4.651586</v>
+        <v>4.693241</v>
       </c>
     </row>
     <row r="25" ht="18" customHeight="1">
@@ -4301,7 +4301,7 @@
         <v>45862.49253582176</v>
       </c>
       <c r="AW25">
-        <v>101.759329</v>
+        <v>101.800984</v>
       </c>
     </row>
     <row r="26" ht="18" customHeight="1">
@@ -4405,7 +4405,7 @@
         <v>45926.59937972222</v>
       </c>
       <c r="AK26">
-        <v>37.652488</v>
+        <v>37.694144</v>
       </c>
     </row>
     <row r="27" ht="18" customHeight="1">
@@ -4506,7 +4506,7 @@
         <v>45959.60018003472</v>
       </c>
       <c r="AK27">
-        <v>4.65169</v>
+        <v>4.693345</v>
       </c>
     </row>
     <row r="28" ht="18" customHeight="1">
@@ -4692,7 +4692,7 @@
         <v>45826.76330768519</v>
       </c>
       <c r="AW28">
-        <v>137.488565</v>
+        <v>137.53022</v>
       </c>
     </row>
     <row r="29" ht="18" customHeight="1">
@@ -4873,7 +4873,7 @@
         <v>45896.58634196759</v>
       </c>
       <c r="AW29">
-        <v>67.665532</v>
+        <v>67.707188</v>
       </c>
     </row>
     <row r="30" ht="18" customHeight="1">
@@ -5051,7 +5051,7 @@
         <v>45905.67982599537</v>
       </c>
       <c r="AW30">
-        <v>58.572049</v>
+        <v>58.613704</v>
       </c>
     </row>
     <row r="31" ht="18" customHeight="1">
@@ -5164,7 +5164,7 @@
         <v>45958.37956106482</v>
       </c>
       <c r="AN31">
-        <v>5.872303</v>
+        <v>5.913958</v>
       </c>
     </row>
     <row r="32" ht="18" customHeight="1">
@@ -5342,7 +5342,7 @@
         <v>45824.67305528936</v>
       </c>
       <c r="AW32">
-        <v>139.578819</v>
+        <v>139.620475</v>
       </c>
     </row>
     <row r="33" ht="18" customHeight="1">
@@ -5523,7 +5523,7 @@
         <v>45888.44432909723</v>
       </c>
       <c r="AW33">
-        <v>75.807535</v>
+        <v>75.84918999999999</v>
       </c>
     </row>
     <row r="34" ht="18" customHeight="1">
@@ -5627,7 +5627,7 @@
         <v>45926.59933546296</v>
       </c>
       <c r="AK34">
-        <v>37.652535</v>
+        <v>37.69419</v>
       </c>
     </row>
     <row r="35" ht="18" customHeight="1">
@@ -5764,7 +5764,7 @@
         <v>45961.42292189815</v>
       </c>
       <c r="AQ35">
-        <v>2.828947</v>
+        <v>2.870602</v>
       </c>
     </row>
     <row r="36" ht="18" customHeight="1">
@@ -5945,7 +5945,7 @@
         <v>45820.33365524306</v>
       </c>
       <c r="AW36">
-        <v>111.639074</v>
+        <v>111.680729</v>
       </c>
     </row>
     <row r="37" ht="18" customHeight="1">
@@ -6123,7 +6123,7 @@
         <v>45860.39854054398</v>
       </c>
       <c r="AW37">
-        <v>103.853333</v>
+        <v>103.894988</v>
       </c>
     </row>
     <row r="38" ht="18" customHeight="1">
@@ -6224,7 +6224,7 @@
         <v>45959.60030722222</v>
       </c>
       <c r="AK38">
-        <v>4.651563</v>
+        <v>4.693218</v>
       </c>
     </row>
     <row r="39" ht="18" customHeight="1">
@@ -6385,7 +6385,7 @@
         <v>45960.48731695602</v>
       </c>
       <c r="AT39">
-        <v>3.764549</v>
+        <v>3.806204</v>
       </c>
     </row>
     <row r="40" ht="18" customHeight="1">
@@ -6486,7 +6486,7 @@
         <v>45959.60010267361</v>
       </c>
       <c r="AK40">
-        <v>4.651771</v>
+        <v>4.693426</v>
       </c>
     </row>
     <row r="41" ht="18" customHeight="1">
@@ -6587,7 +6587,7 @@
         <v>45959.60038484954</v>
       </c>
       <c r="AK41">
-        <v>4.651481</v>
+        <v>4.693137</v>
       </c>
     </row>
     <row r="42" ht="18" customHeight="1">
@@ -6688,7 +6688,7 @@
         <v>45959.60041594907</v>
       </c>
       <c r="AK42">
-        <v>4.651458</v>
+        <v>4.693113</v>
       </c>
     </row>
     <row r="43" ht="18" customHeight="1">
@@ -6827,7 +6827,7 @@
         <v>45954.64844130787</v>
       </c>
       <c r="AQ43">
-        <v>9.603426000000001</v>
+        <v>9.645080999999999</v>
       </c>
     </row>
     <row r="44" ht="18" customHeight="1">
@@ -7008,7 +7008,7 @@
         <v>45888.44494424769</v>
       </c>
       <c r="AW44">
-        <v>75.806921</v>
+        <v>75.84857599999999</v>
       </c>
     </row>
     <row r="45" ht="18" customHeight="1">
@@ -7189,7 +7189,7 @@
         <v>45903.36153759259</v>
       </c>
       <c r="AW45">
-        <v>60.890336</v>
+        <v>60.931991</v>
       </c>
     </row>
     <row r="46" ht="18" customHeight="1">
@@ -7373,7 +7373,7 @@
         <v>45924.33465340278</v>
       </c>
       <c r="AW46">
-        <v>26.923692</v>
+        <v>26.965347</v>
       </c>
     </row>
     <row r="47" ht="18" customHeight="1">
@@ -7554,7 +7554,7 @@
         <v>45937.3293883912</v>
       </c>
       <c r="AW47">
-        <v>26.922477</v>
+        <v>26.964132</v>
       </c>
     </row>
     <row r="48" ht="18" customHeight="1">
@@ -7655,7 +7655,7 @@
         <v>45937.55079829862</v>
       </c>
       <c r="AK48">
-        <v>26.701076</v>
+        <v>26.742731</v>
       </c>
     </row>
     <row r="49" ht="18" customHeight="1">
@@ -7836,7 +7836,7 @@
         <v>45860.39754922454</v>
       </c>
       <c r="AW49">
-        <v>103.854317</v>
+        <v>103.895972</v>
       </c>
     </row>
     <row r="50" ht="18" customHeight="1">
@@ -8014,7 +8014,7 @@
         <v>45859.70404015046</v>
       </c>
       <c r="AW50">
-        <v>104.547824</v>
+        <v>104.589479</v>
       </c>
     </row>
     <row r="51" ht="18" customHeight="1">
@@ -8195,7 +8195,7 @@
         <v>45846.48855997685</v>
       </c>
       <c r="AW51">
-        <v>117.76331</v>
+        <v>117.804965</v>
       </c>
     </row>
     <row r="52" ht="18" customHeight="1">
@@ -8379,7 +8379,7 @@
         <v>45946.6547500926</v>
       </c>
       <c r="AW52">
-        <v>11.69044</v>
+        <v>11.732095</v>
       </c>
     </row>
     <row r="53" ht="18" customHeight="1">
@@ -8480,7 +8480,7 @@
         <v>45961.44066628473</v>
       </c>
       <c r="AK53">
-        <v>2.811204</v>
+        <v>2.852859</v>
       </c>
     </row>
     <row r="54" ht="18" customHeight="1">
@@ -8664,7 +8664,7 @@
         <v>45868.73102224537</v>
       </c>
       <c r="AW54">
-        <v>95.52084499999999</v>
+        <v>95.5625</v>
       </c>
     </row>
     <row r="55" ht="18" customHeight="1">
@@ -8842,7 +8842,7 @@
         <v>45821.6263675</v>
       </c>
       <c r="AW55">
-        <v>142.625498</v>
+        <v>142.667153</v>
       </c>
     </row>
     <row r="56" ht="18" customHeight="1">
@@ -9020,7 +9020,7 @@
         <v>45831.57755690972</v>
       </c>
       <c r="AW56">
-        <v>132.674317</v>
+        <v>132.715972</v>
       </c>
     </row>
     <row r="57" ht="18" customHeight="1">
@@ -9121,7 +9121,7 @@
         <v>45936.75055488426</v>
       </c>
       <c r="AK57">
-        <v>27.501319</v>
+        <v>27.542975</v>
       </c>
     </row>
     <row r="58" ht="18" customHeight="1">
@@ -9299,7 +9299,7 @@
         <v>45859.70488313658</v>
       </c>
       <c r="AW58">
-        <v>104.546991</v>
+        <v>104.588646</v>
       </c>
     </row>
     <row r="59" ht="18" customHeight="1">
@@ -9460,7 +9460,7 @@
         <v>45958.41020675926</v>
       </c>
       <c r="AT59">
-        <v>5.841667</v>
+        <v>5.883322</v>
       </c>
     </row>
     <row r="60" ht="18" customHeight="1">
@@ -9599,7 +9599,7 @@
         <v>45954.64892450231</v>
       </c>
       <c r="AQ60">
-        <v>9.60294</v>
+        <v>9.644595000000001</v>
       </c>
     </row>
     <row r="61" ht="18" customHeight="1">
@@ -9777,7 +9777,7 @@
         <v>45856.44919015047</v>
       </c>
       <c r="AW61">
-        <v>107.802674</v>
+        <v>107.844329</v>
       </c>
     </row>
     <row r="62" ht="18" customHeight="1">
@@ -9955,7 +9955,7 @@
         <v>45895.64805509259</v>
       </c>
       <c r="AW62">
-        <v>68.603819</v>
+        <v>68.645475</v>
       </c>
     </row>
     <row r="63" ht="18" customHeight="1">
@@ -10136,7 +10136,7 @@
         <v>45923.70330438657</v>
       </c>
       <c r="AW63">
-        <v>40.548565</v>
+        <v>40.59022</v>
       </c>
     </row>
     <row r="64" ht="18" customHeight="1">
@@ -10249,7 +10249,7 @@
         <v>45947.74647541667</v>
       </c>
       <c r="AN64">
-        <v>16.505394</v>
+        <v>16.547049</v>
       </c>
     </row>
     <row r="65" ht="18" customHeight="1">
@@ -10427,7 +10427,7 @@
         <v>45820.33324042824</v>
       </c>
       <c r="AW65">
-        <v>143.918634</v>
+        <v>143.960289</v>
       </c>
     </row>
     <row r="66" ht="18" customHeight="1">
@@ -10605,7 +10605,7 @@
         <v>45817.44034118055</v>
       </c>
       <c r="AW66">
-        <v>146.811528</v>
+        <v>146.853183</v>
       </c>
     </row>
     <row r="67" ht="18" customHeight="1">
@@ -10783,7 +10783,7 @@
         <v>45859.68910778935</v>
       </c>
       <c r="AW67">
-        <v>104.562766</v>
+        <v>104.604421</v>
       </c>
     </row>
     <row r="68" ht="18" customHeight="1">
@@ -10884,7 +10884,7 @@
         <v>45937.55070907407</v>
       </c>
       <c r="AK68">
-        <v>26.701157</v>
+        <v>26.742813</v>
       </c>
     </row>
     <row r="69" ht="18" customHeight="1">
@@ -11065,7 +11065,7 @@
         <v>45902.58757359954</v>
       </c>
       <c r="AW69">
-        <v>61.664294</v>
+        <v>61.705949</v>
       </c>
     </row>
     <row r="70" ht="18" customHeight="1">
@@ -11246,7 +11246,7 @@
         <v>45959.55501203703</v>
       </c>
       <c r="AW70">
-        <v>4.696852</v>
+        <v>4.738507</v>
       </c>
     </row>
     <row r="71" ht="18" customHeight="1">
@@ -11347,7 +11347,7 @@
         <v>45959.60036175927</v>
       </c>
       <c r="AK71">
-        <v>4.651505</v>
+        <v>4.69316</v>
       </c>
     </row>
     <row r="72" ht="18" customHeight="1">
@@ -11489,7 +11489,7 @@
         <v>45953.71854960648</v>
       </c>
       <c r="AQ72">
-        <v>10.597118</v>
+        <v>10.638773</v>
       </c>
     </row>
     <row r="73" ht="18" customHeight="1">
@@ -11590,7 +11590,7 @@
         <v>45959.6001238426</v>
       </c>
       <c r="AK73">
-        <v>4.651748</v>
+        <v>4.693403</v>
       </c>
     </row>
     <row r="74" ht="18" customHeight="1">
@@ -11776,7 +11776,7 @@
         <v>45845.61766498843</v>
       </c>
       <c r="AW74">
-        <v>118.634201</v>
+        <v>118.675856</v>
       </c>
     </row>
     <row r="75" ht="18" customHeight="1">
@@ -11954,7 +11954,7 @@
         <v>45908.5914516551</v>
       </c>
       <c r="AW75">
-        <v>55.660417</v>
+        <v>55.702072</v>
       </c>
     </row>
     <row r="76" ht="18" customHeight="1">
@@ -12064,7 +12064,7 @@
         <v>45947.74104872685</v>
       </c>
       <c r="AN76">
-        <v>16.510822</v>
+        <v>16.552477</v>
       </c>
     </row>
     <row r="77" ht="18" customHeight="1">
@@ -12168,7 +12168,7 @@
         <v>45908.54209915509</v>
       </c>
       <c r="AK77">
-        <v>55.709769</v>
+        <v>55.751424</v>
       </c>
     </row>
     <row r="78" ht="18" customHeight="1">
@@ -12352,7 +12352,7 @@
         <v>45894.4102940162</v>
       </c>
       <c r="AW78">
-        <v>59.869063</v>
+        <v>59.910718</v>
       </c>
     </row>
     <row r="79" ht="18" customHeight="1">
@@ -12533,7 +12533,7 @@
         <v>45831.57415840278</v>
       </c>
       <c r="AW79">
-        <v>132.677708</v>
+        <v>132.719363</v>
       </c>
     </row>
     <row r="80" ht="18" customHeight="1">
@@ -12711,7 +12711,7 @@
         <v>45952.41303611111</v>
       </c>
       <c r="AW80">
-        <v>11.838831</v>
+        <v>11.880486</v>
       </c>
     </row>
     <row r="81" ht="18" customHeight="1">
@@ -12892,7 +12892,7 @@
         <v>45937.3283994213</v>
       </c>
       <c r="AW81">
-        <v>26.923472</v>
+        <v>26.965127</v>
       </c>
     </row>
     <row r="82" ht="18" customHeight="1">
@@ -13073,7 +13073,7 @@
         <v>45957.71828232639</v>
       </c>
       <c r="AW82">
-        <v>6.533588</v>
+        <v>6.575243</v>
       </c>
     </row>
     <row r="83" ht="18" customHeight="1">
@@ -13215,7 +13215,7 @@
         <v>45961.4227958449</v>
       </c>
       <c r="AQ83">
-        <v>2.829074</v>
+        <v>2.870729</v>
       </c>
     </row>
     <row r="84" ht="18" customHeight="1">
@@ -13393,7 +13393,7 @@
         <v>45852.54883409722</v>
       </c>
       <c r="AW84">
-        <v>111.703032</v>
+        <v>111.744688</v>
       </c>
     </row>
     <row r="85" ht="18" customHeight="1">
@@ -13571,7 +13571,7 @@
         <v>45821.67408983796</v>
       </c>
       <c r="AW85">
-        <v>142.577778</v>
+        <v>142.619433</v>
       </c>
     </row>
     <row r="86" ht="18" customHeight="1">
@@ -13760,7 +13760,7 @@
         <v>45873.70541589121</v>
       </c>
       <c r="AW86">
-        <v>90.547442</v>
+        <v>90.589097</v>
       </c>
     </row>
     <row r="87" ht="18" customHeight="1">
@@ -13941,7 +13941,7 @@
         <v>45904.38451509259</v>
       </c>
       <c r="AW87">
-        <v>59.86735</v>
+        <v>59.909005</v>
       </c>
     </row>
     <row r="88" ht="18" customHeight="1">
@@ -14122,7 +14122,7 @@
         <v>45923.7104591088</v>
       </c>
       <c r="AW88">
-        <v>40.541412</v>
+        <v>40.583067</v>
       </c>
     </row>
     <row r="89" ht="18" customHeight="1">
@@ -14261,7 +14261,7 @@
         <v>45939.61865349537</v>
       </c>
       <c r="AQ89">
-        <v>24.633218</v>
+        <v>24.674873</v>
       </c>
     </row>
     <row r="90" ht="18" customHeight="1">
@@ -14442,7 +14442,7 @@
         <v>45817.66125234954</v>
       </c>
       <c r="AW90">
-        <v>96.549954</v>
+        <v>96.59160900000001</v>
       </c>
     </row>
     <row r="91" ht="18" customHeight="1">
@@ -14620,7 +14620,7 @@
         <v>45826.76919975695</v>
       </c>
       <c r="AW91">
-        <v>137.482674</v>
+        <v>137.524329</v>
       </c>
     </row>
     <row r="92" ht="18" customHeight="1">
@@ -14798,7 +14798,7 @@
         <v>45917.32877043981</v>
       </c>
       <c r="AW92">
-        <v>46.923102</v>
+        <v>46.964757</v>
       </c>
     </row>
     <row r="93" ht="18" customHeight="1">
@@ -14976,7 +14976,7 @@
         <v>45859.7056584838</v>
       </c>
       <c r="AW93">
-        <v>104.546215</v>
+        <v>104.58787</v>
       </c>
     </row>
     <row r="94" ht="18" customHeight="1">
@@ -15077,7 +15077,7 @@
         <v>45959.60045502314</v>
       </c>
       <c r="AK94">
-        <v>4.651412</v>
+        <v>4.693067</v>
       </c>
     </row>
     <row r="95" ht="18" customHeight="1">
@@ -15255,7 +15255,7 @@
         <v>45820.33284418982</v>
       </c>
       <c r="AW95">
-        <v>143.919028</v>
+        <v>143.960683</v>
       </c>
     </row>
     <row r="96" ht="18" customHeight="1">
@@ -15433,7 +15433,7 @@
         <v>45908.71817314815</v>
       </c>
       <c r="AW96">
-        <v>55.533692</v>
+        <v>55.575347</v>
       </c>
     </row>
     <row r="97" ht="18" customHeight="1">
@@ -15572,7 +15572,7 @@
         <v>45954.64821246528</v>
       </c>
       <c r="AQ97">
-        <v>9.603657</v>
+        <v>9.645313</v>
       </c>
     </row>
     <row r="98" ht="18" customHeight="1">
@@ -15753,7 +15753,7 @@
         <v>45890.64899726852</v>
       </c>
       <c r="AW98">
-        <v>73.60287</v>
+        <v>73.644525</v>
       </c>
     </row>
     <row r="99" ht="18" customHeight="1">
@@ -15934,7 +15934,7 @@
         <v>45898.57314238426</v>
       </c>
       <c r="AW99">
-        <v>65.67872699999999</v>
+        <v>65.720382</v>
       </c>
     </row>
     <row r="100" ht="18" customHeight="1">
@@ -16112,7 +16112,7 @@
         <v>45824.58323728009</v>
       </c>
       <c r="AW100">
-        <v>139.668634</v>
+        <v>139.710289</v>
       </c>
     </row>
     <row r="101" ht="18" customHeight="1">
@@ -16293,7 +16293,7 @@
         <v>45868.58624710648</v>
       </c>
       <c r="AW101">
-        <v>95.66562500000001</v>
+        <v>95.70728</v>
       </c>
     </row>
     <row r="102" ht="18" customHeight="1">
@@ -16477,7 +16477,7 @@
         <v>45875.68373804398</v>
       </c>
       <c r="AW102">
-        <v>34.924375</v>
+        <v>34.96603</v>
       </c>
     </row>
     <row r="103" ht="18" customHeight="1">
@@ -16578,7 +16578,7 @@
         <v>45936.75048913194</v>
       </c>
       <c r="AK103">
-        <v>27.501377</v>
+        <v>27.543032</v>
       </c>
     </row>
     <row r="104" ht="18" customHeight="1">
@@ -16682,7 +16682,7 @@
         <v>45926.59938667824</v>
       </c>
       <c r="AK104">
-        <v>37.652477</v>
+        <v>37.694132</v>
       </c>
     </row>
     <row r="105" ht="18" customHeight="1">
@@ -16863,7 +16863,7 @@
         <v>45908.66222837963</v>
       </c>
       <c r="AW105">
-        <v>55.589641</v>
+        <v>55.631296</v>
       </c>
     </row>
     <row r="106" ht="18" customHeight="1">
@@ -17044,7 +17044,7 @@
         <v>45817.43553984954</v>
       </c>
       <c r="AW106">
-        <v>94.10250000000001</v>
+        <v>94.144155</v>
       </c>
     </row>
     <row r="107" ht="18" customHeight="1">
@@ -17225,7 +17225,7 @@
         <v>45861.50585359953</v>
       </c>
       <c r="AW107">
-        <v>102.746019</v>
+        <v>102.787674</v>
       </c>
     </row>
     <row r="108" ht="18" customHeight="1">
@@ -17329,7 +17329,7 @@
         <v>45908.53444716435</v>
       </c>
       <c r="AK108">
-        <v>55.717419</v>
+        <v>55.759074</v>
       </c>
     </row>
     <row r="109" ht="18" customHeight="1">
@@ -17430,7 +17430,7 @@
         <v>45959.60023207176</v>
       </c>
       <c r="AK109">
-        <v>4.651632</v>
+        <v>4.693287</v>
       </c>
     </row>
     <row r="110" ht="18" customHeight="1">
@@ -17531,7 +17531,7 @@
         <v>45959.60042334491</v>
       </c>
       <c r="AK110">
-        <v>4.651447</v>
+        <v>4.693102</v>
       </c>
     </row>
     <row r="111" ht="18" customHeight="1">
@@ -17712,7 +17712,7 @@
         <v>45959.57354159722</v>
       </c>
       <c r="AW111">
-        <v>4.678333</v>
+        <v>4.719988</v>
       </c>
     </row>
     <row r="112" ht="18" customHeight="1">
@@ -17890,7 +17890,7 @@
         <v>45817.43738373843</v>
       </c>
       <c r="AW112">
-        <v>146.814491</v>
+        <v>146.856146</v>
       </c>
     </row>
     <row r="113" ht="18" customHeight="1">
@@ -18071,7 +18071,7 @@
         <v>45821.67595234954</v>
       </c>
       <c r="AW113">
-        <v>142.575914</v>
+        <v>142.617569</v>
       </c>
     </row>
     <row r="114" ht="18" customHeight="1">
@@ -18249,7 +18249,7 @@
         <v>45831.62649351852</v>
       </c>
       <c r="AW114">
-        <v>132.62537</v>
+        <v>132.667025</v>
       </c>
     </row>
     <row r="115" ht="18" customHeight="1">
@@ -18430,7 +18430,7 @@
         <v>45929.32908571759</v>
       </c>
       <c r="AW115">
-        <v>34.922778</v>
+        <v>34.964433</v>
       </c>
     </row>
     <row r="116" ht="18" customHeight="1">
@@ -18534,7 +18534,7 @@
         <v>45926.59937309028</v>
       </c>
       <c r="AK116">
-        <v>37.6525</v>
+        <v>37.694155</v>
       </c>
     </row>
     <row r="117" ht="18" customHeight="1">
@@ -18715,7 +18715,7 @@
         <v>45957.72764497685</v>
       </c>
       <c r="AW117">
-        <v>6.524225</v>
+        <v>6.56588</v>
       </c>
     </row>
     <row r="118" ht="18" customHeight="1">
@@ -18893,7 +18893,7 @@
         <v>45890.69579123842</v>
       </c>
       <c r="AW118">
-        <v>73.556076</v>
+        <v>73.597731</v>
       </c>
     </row>
     <row r="119" ht="18" customHeight="1">
@@ -19074,7 +19074,7 @@
         <v>45842.7072899537</v>
       </c>
       <c r="AW119">
-        <v>121.544583</v>
+        <v>121.586238</v>
       </c>
     </row>
     <row r="120" ht="18" customHeight="1">
@@ -19258,7 +19258,7 @@
         <v>45868.56623082176</v>
       </c>
       <c r="AW120">
-        <v>95.685637</v>
+        <v>95.72729200000001</v>
       </c>
     </row>
     <row r="121" ht="18" customHeight="1">
@@ -19439,7 +19439,7 @@
         <v>45904.38667092593</v>
       </c>
       <c r="AW121">
-        <v>59.865197</v>
+        <v>59.906852</v>
       </c>
     </row>
     <row r="122" ht="18" customHeight="1">
@@ -19540,7 +19540,7 @@
         <v>45936.75044380788</v>
       </c>
       <c r="AK122">
-        <v>27.501424</v>
+        <v>27.543079</v>
       </c>
     </row>
     <row r="123" ht="18" customHeight="1">
@@ -19641,7 +19641,7 @@
         <v>45959.60029184028</v>
       </c>
       <c r="AK123">
-        <v>4.651574</v>
+        <v>4.693229</v>
       </c>
     </row>
     <row r="124" ht="18" customHeight="1">
@@ -19819,7 +19819,7 @@
         <v>45826.76858534722</v>
       </c>
       <c r="AW124">
-        <v>137.483287</v>
+        <v>137.524942</v>
       </c>
     </row>
     <row r="125" ht="18" customHeight="1">
@@ -19920,7 +19920,7 @@
         <v>45936.74724322917</v>
       </c>
       <c r="AK125">
-        <v>27.50463</v>
+        <v>27.546285</v>
       </c>
     </row>
     <row r="126" ht="18" customHeight="1">
@@ -20021,7 +20021,7 @@
         <v>45959.60039233796</v>
       </c>
       <c r="AK126">
-        <v>4.651481</v>
+        <v>4.693137</v>
       </c>
     </row>
     <row r="127" ht="18" customHeight="1">
@@ -20194,7 +20194,7 @@
         <v>45831.67398204861</v>
       </c>
       <c r="AW127">
-        <v>132.577882</v>
+        <v>132.619537</v>
       </c>
     </row>
     <row r="128" ht="18" customHeight="1">
@@ -20295,7 +20295,7 @@
         <v>45937.55068216435</v>
       </c>
       <c r="AK128">
-        <v>26.701192</v>
+        <v>26.742847</v>
       </c>
     </row>
     <row r="129" ht="18" customHeight="1">
@@ -20396,7 +20396,7 @@
         <v>45959.60040799768</v>
       </c>
       <c r="AK129">
-        <v>4.651458</v>
+        <v>4.693113</v>
       </c>
     </row>
     <row r="130" ht="18" customHeight="1">
@@ -20577,7 +20577,7 @@
         <v>45917.46641751158</v>
       </c>
       <c r="AW130">
-        <v>46.785451</v>
+        <v>46.827106</v>
       </c>
     </row>
     <row r="131" ht="18" customHeight="1">
@@ -20758,7 +20758,7 @@
         <v>45923.31500230324</v>
       </c>
       <c r="AW131">
-        <v>40.936863</v>
+        <v>40.978519</v>
       </c>
     </row>
     <row r="132" ht="18" customHeight="1">
@@ -20936,7 +20936,7 @@
         <v>45812.58332680556</v>
       </c>
       <c r="AW132">
-        <v>150.627905</v>
+        <v>150.66956</v>
       </c>
     </row>
     <row r="133" ht="18" customHeight="1">
@@ -21114,7 +21114,7 @@
         <v>45887.78360177083</v>
       </c>
       <c r="AW133">
-        <v>76.468264</v>
+        <v>76.509919</v>
       </c>
     </row>
     <row r="134" ht="18" customHeight="1">
@@ -21295,7 +21295,7 @@
         <v>45929.32963659722</v>
       </c>
       <c r="AW134">
-        <v>34.922234</v>
+        <v>34.963889</v>
       </c>
     </row>
     <row r="135" ht="18" customHeight="1">
@@ -21438,7 +21438,7 @@
         <v>45939.61855898148</v>
       </c>
       <c r="AN135">
-        <v>11.706794</v>
+        <v>11.748449</v>
       </c>
       <c r="AO135" s="2">
         <v>45939.6185591088</v>
@@ -21548,7 +21548,7 @@
         <v>45959.6003153588</v>
       </c>
       <c r="AK136">
-        <v>4.651551</v>
+        <v>4.693206</v>
       </c>
     </row>
     <row r="137" ht="18" customHeight="1">
@@ -21726,7 +21726,7 @@
         <v>45831.62328704861</v>
       </c>
       <c r="AW137">
-        <v>132.628576</v>
+        <v>132.670231</v>
       </c>
     </row>
     <row r="138" ht="18" customHeight="1">
@@ -21904,7 +21904,7 @@
         <v>45826.76692778935</v>
       </c>
       <c r="AW138">
-        <v>137.484942</v>
+        <v>137.526597</v>
       </c>
     </row>
     <row r="139" ht="18" customHeight="1">
@@ -22085,7 +22085,7 @@
         <v>45890.58630611112</v>
       </c>
       <c r="AW139">
-        <v>73.665567</v>
+        <v>73.707222</v>
       </c>
     </row>
     <row r="140" ht="18" customHeight="1">
@@ -22186,7 +22186,7 @@
         <v>45959.60037689815</v>
       </c>
       <c r="AK140">
-        <v>4.651493</v>
+        <v>4.693148</v>
       </c>
     </row>
     <row r="141" ht="18" customHeight="1">
@@ -22364,7 +22364,7 @@
         <v>45856.44962944444</v>
       </c>
       <c r="AW141">
-        <v>107.802245</v>
+        <v>107.8439</v>
       </c>
     </row>
     <row r="142" ht="18" customHeight="1">
@@ -22542,7 +22542,7 @@
         <v>45859.70515091435</v>
       </c>
       <c r="AW142">
-        <v>104.546713</v>
+        <v>104.588368</v>
       </c>
     </row>
     <row r="143" ht="18" customHeight="1">
@@ -22723,7 +22723,7 @@
         <v>45896.58530709491</v>
       </c>
       <c r="AW143">
-        <v>67.666563</v>
+        <v>67.708218</v>
       </c>
     </row>
     <row r="144" ht="18" customHeight="1">
@@ -22824,7 +22824,7 @@
         <v>45959.60013854166</v>
       </c>
       <c r="AK144">
-        <v>4.651736</v>
+        <v>4.693391</v>
       </c>
     </row>
     <row r="145" ht="18" customHeight="1">
@@ -23005,7 +23005,7 @@
         <v>45924.65307170139</v>
       </c>
       <c r="AW145">
-        <v>39.598796</v>
+        <v>39.640451</v>
       </c>
     </row>
     <row r="146" ht="18" customHeight="1">
@@ -23186,7 +23186,7 @@
         <v>45924.45313572917</v>
       </c>
       <c r="AW146">
-        <v>39.798738</v>
+        <v>39.840394</v>
       </c>
     </row>
     <row r="147" ht="18" customHeight="1">
@@ -23328,7 +23328,7 @@
         <v>45939.61876168981</v>
       </c>
       <c r="AQ147">
-        <v>24.633102</v>
+        <v>24.674757</v>
       </c>
     </row>
     <row r="148" ht="18" customHeight="1">
@@ -23509,7 +23509,7 @@
         <v>45905.60530078704</v>
       </c>
       <c r="AW148">
-        <v>61.496933</v>
+        <v>61.538588</v>
       </c>
     </row>
     <row r="149" ht="18" customHeight="1">
@@ -23698,7 +23698,7 @@
         <v>45912.68970434028</v>
       </c>
       <c r="AW149">
-        <v>51.562164</v>
+        <v>51.603819</v>
       </c>
     </row>
     <row r="150" ht="18" customHeight="1">
@@ -23866,7 +23866,7 @@
         <v>45882.61953023148</v>
       </c>
       <c r="AW150">
-        <v>81.632338</v>
+        <v>81.673993</v>
       </c>
     </row>
     <row r="151" ht="18" customHeight="1">
@@ -24047,7 +24047,7 @@
         <v>45929.33033346065</v>
       </c>
       <c r="AW151">
-        <v>34.921539</v>
+        <v>34.963194</v>
       </c>
     </row>
     <row r="152" ht="18" customHeight="1">
@@ -24186,7 +24186,7 @@
         <v>45947.63865299769</v>
       </c>
       <c r="AQ152">
-        <v>16.613218</v>
+        <v>16.654873</v>
       </c>
     </row>
     <row r="153" ht="18" customHeight="1">
@@ -24287,7 +24287,7 @@
         <v>45959.60027336805</v>
       </c>
       <c r="AK153">
-        <v>4.651597</v>
+        <v>4.693252</v>
       </c>
     </row>
     <row r="154" ht="18" customHeight="1">
@@ -24468,7 +24468,7 @@
         <v>45860.39774737268</v>
       </c>
       <c r="AW154">
-        <v>103.85412</v>
+        <v>103.895775</v>
       </c>
     </row>
     <row r="155" ht="18" customHeight="1">
@@ -24649,7 +24649,7 @@
         <v>45904.38106203704</v>
       </c>
       <c r="AW155">
-        <v>59.87081</v>
+        <v>59.912465</v>
       </c>
     </row>
     <row r="156" ht="18" customHeight="1">
@@ -24756,7 +24756,7 @@
         <v>45909.6343971412</v>
       </c>
       <c r="AK156">
-        <v>55.703519</v>
+        <v>55.745174</v>
       </c>
       <c r="AL156" s="2">
         <v>45909.63439736111</v>
@@ -24943,7 +24943,7 @@
         <v>45870.37493769676</v>
       </c>
       <c r="AW157">
-        <v>93.87693299999999</v>
+        <v>93.918588</v>
       </c>
     </row>
     <row r="158" ht="18" customHeight="1">
@@ -25124,7 +25124,7 @@
         <v>45954.62848792824</v>
       </c>
       <c r="AW158">
-        <v>9.623379999999999</v>
+        <v>9.665035</v>
       </c>
     </row>
     <row r="159" ht="18" customHeight="1">
@@ -25225,7 +25225,7 @@
         <v>45959.60013106481</v>
       </c>
       <c r="AK159">
-        <v>4.651736</v>
+        <v>4.693391</v>
       </c>
     </row>
     <row r="160" ht="18" customHeight="1">
@@ -25403,7 +25403,7 @@
         <v>45821.67315659721</v>
       </c>
       <c r="AW160">
-        <v>142.578715</v>
+        <v>142.62037</v>
       </c>
     </row>
     <row r="161" ht="18" customHeight="1">
@@ -25584,7 +25584,7 @@
         <v>45845.32285525464</v>
       </c>
       <c r="AW161">
-        <v>118.929016</v>
+        <v>118.970671</v>
       </c>
     </row>
     <row r="162" ht="18" customHeight="1">
@@ -25757,7 +25757,7 @@
         <v>45905.68003464121</v>
       </c>
       <c r="AW162">
-        <v>58.57184</v>
+        <v>58.613495</v>
       </c>
     </row>
     <row r="163" ht="18" customHeight="1">
@@ -25858,7 +25858,7 @@
         <v>45959.60044730324</v>
       </c>
       <c r="AK163">
-        <v>4.651424</v>
+        <v>4.693079</v>
       </c>
     </row>
     <row r="164" ht="18" customHeight="1">
@@ -26036,7 +26036,7 @@
         <v>45870.3699896875</v>
       </c>
       <c r="AW164">
-        <v>93.88187499999999</v>
+        <v>93.92353</v>
       </c>
     </row>
     <row r="165" ht="18" customHeight="1">
@@ -26214,7 +26214,7 @@
         <v>45817.43698824074</v>
       </c>
       <c r="AW165">
-        <v>146.814884</v>
+        <v>146.856539</v>
       </c>
     </row>
     <row r="166" ht="18" customHeight="1">
@@ -26392,7 +26392,7 @@
         <v>45895.66891309028</v>
       </c>
       <c r="AW166">
-        <v>68.58295099999999</v>
+        <v>68.624606</v>
       </c>
     </row>
     <row r="167" ht="18" customHeight="1">
@@ -26570,7 +26570,7 @@
         <v>45824.67360026621</v>
       </c>
       <c r="AW167">
-        <v>139.578264</v>
+        <v>139.619919</v>
       </c>
     </row>
     <row r="168" ht="18" customHeight="1">
@@ -26748,7 +26748,7 @@
         <v>45833.56676576388</v>
       </c>
       <c r="AW168">
-        <v>130.685104</v>
+        <v>130.726759</v>
       </c>
     </row>
     <row r="169" ht="18" customHeight="1">
@@ -26926,7 +26926,7 @@
         <v>45895.64817069445</v>
       </c>
       <c r="AW169">
-        <v>68.60370399999999</v>
+        <v>68.645359</v>
       </c>
     </row>
     <row r="170" ht="18" customHeight="1">
@@ -27027,7 +27027,7 @@
         <v>45937.55080626157</v>
       </c>
       <c r="AK170">
-        <v>26.701065</v>
+        <v>26.74272</v>
       </c>
     </row>
     <row r="171" ht="18" customHeight="1">
@@ -27169,7 +27169,7 @@
         <v>45960.7374919213</v>
       </c>
       <c r="AQ171">
-        <v>3.514375</v>
+        <v>3.55603</v>
       </c>
     </row>
     <row r="172" ht="18" customHeight="1">
@@ -27350,7 +27350,7 @@
         <v>45890.75601248843</v>
       </c>
       <c r="AW172">
-        <v>73.495856</v>
+        <v>73.53751200000001</v>
       </c>
     </row>
     <row r="173" ht="18" customHeight="1">
@@ -27528,7 +27528,7 @@
         <v>45824.67396405093</v>
       </c>
       <c r="AW173">
-        <v>139.577905</v>
+        <v>139.61956</v>
       </c>
     </row>
     <row r="174" ht="18" customHeight="1">
@@ -27709,7 +27709,7 @@
         <v>45868.57042331019</v>
       </c>
       <c r="AW174">
-        <v>95.68144700000001</v>
+        <v>95.723102</v>
       </c>
     </row>
     <row r="175" ht="18" customHeight="1">
@@ -27890,7 +27890,7 @@
         <v>45923.31572024305</v>
       </c>
       <c r="AW175">
-        <v>40.936146</v>
+        <v>40.977801</v>
       </c>
     </row>
     <row r="176" ht="18" customHeight="1">
@@ -27994,7 +27994,7 @@
         <v>45926.59931493056</v>
       </c>
       <c r="AK176">
-        <v>37.652558</v>
+        <v>37.694213</v>
       </c>
     </row>
     <row r="177" ht="18" customHeight="1">
@@ -28172,7 +28172,7 @@
         <v>45817.4294139699</v>
       </c>
       <c r="AW177">
-        <v>146.822454</v>
+        <v>146.864109</v>
       </c>
     </row>
     <row r="178" ht="18" customHeight="1">
@@ -28340,7 +28340,7 @@
         <v>45882.60734775463</v>
       </c>
       <c r="AW178">
-        <v>81.644525</v>
+        <v>81.686181</v>
       </c>
     </row>
     <row r="179" ht="18" customHeight="1">
@@ -28524,7 +28524,7 @@
         <v>45868.56660532407</v>
       </c>
       <c r="AW179">
-        <v>95.685266</v>
+        <v>95.726921</v>
       </c>
     </row>
     <row r="180" ht="18" customHeight="1">
@@ -28625,7 +28625,7 @@
         <v>45937.55067289351</v>
       </c>
       <c r="AK180">
-        <v>26.701192</v>
+        <v>26.742847</v>
       </c>
     </row>
     <row r="181" ht="18" customHeight="1">
@@ -28806,7 +28806,7 @@
         <v>45904.38355210648</v>
       </c>
       <c r="AW181">
-        <v>59.868322</v>
+        <v>59.909977</v>
       </c>
     </row>
     <row r="182" ht="18" customHeight="1">
@@ -28990,7 +28990,7 @@
         <v>45905.68527717593</v>
       </c>
       <c r="AW182">
-        <v>40.939688</v>
+        <v>40.981343</v>
       </c>
     </row>
     <row r="183" ht="18" customHeight="1">
@@ -29091,7 +29091,7 @@
         <v>45959.60029939815</v>
       </c>
       <c r="AK183">
-        <v>4.651574</v>
+        <v>4.693229</v>
       </c>
     </row>
     <row r="184" ht="18" customHeight="1">
@@ -29269,7 +29269,7 @@
         <v>45810.36211870371</v>
       </c>
       <c r="AW184">
-        <v>153.889745</v>
+        <v>153.9314</v>
       </c>
     </row>
     <row r="185" ht="18" customHeight="1">
@@ -29447,7 +29447,7 @@
         <v>45824.58295356482</v>
       </c>
       <c r="AW185">
-        <v>139.668912</v>
+        <v>139.710567</v>
       </c>
     </row>
     <row r="186" ht="18" customHeight="1">
@@ -29628,7 +29628,7 @@
         <v>45904.37770018518</v>
       </c>
       <c r="AW186">
-        <v>59.874167</v>
+        <v>59.915822</v>
       </c>
     </row>
     <row r="187" ht="18" customHeight="1">
@@ -29806,7 +29806,7 @@
         <v>45930.59030788194</v>
       </c>
       <c r="AW187">
-        <v>33.661563</v>
+        <v>33.703218</v>
       </c>
     </row>
     <row r="188" ht="18" customHeight="1">
@@ -29987,7 +29987,7 @@
         <v>45810.35108107638</v>
       </c>
       <c r="AW188">
-        <v>126.905451</v>
+        <v>126.947106</v>
       </c>
     </row>
     <row r="189" ht="18" customHeight="1">
@@ -30165,7 +30165,7 @@
         <v>45826.76801165509</v>
       </c>
       <c r="AW189">
-        <v>137.483854</v>
+        <v>137.525509</v>
       </c>
     </row>
     <row r="190" ht="18" customHeight="1">
@@ -30343,7 +30343,7 @@
         <v>45898.66446734954</v>
       </c>
       <c r="AW190">
-        <v>65.587407</v>
+        <v>65.629063</v>
       </c>
     </row>
     <row r="191" ht="18" customHeight="1">
@@ -30524,7 +30524,7 @@
         <v>45842.71044888889</v>
       </c>
       <c r="AW191">
-        <v>121.541424</v>
+        <v>121.583079</v>
       </c>
     </row>
     <row r="192" ht="18" customHeight="1">
@@ -30705,7 +30705,7 @@
         <v>45880.49447488426</v>
       </c>
       <c r="AW192">
-        <v>69.510845</v>
+        <v>69.55249999999999</v>
       </c>
     </row>
     <row r="193" ht="18" customHeight="1">
@@ -30883,7 +30883,7 @@
         <v>45821.69981792824</v>
       </c>
       <c r="AW193">
-        <v>142.552049</v>
+        <v>142.593704</v>
       </c>
     </row>
     <row r="194" ht="18" customHeight="1">
@@ -31061,7 +31061,7 @@
         <v>45824.58350305556</v>
       </c>
       <c r="AW194">
-        <v>139.668368</v>
+        <v>139.710023</v>
       </c>
     </row>
     <row r="195" ht="18" customHeight="1">
@@ -31239,7 +31239,7 @@
         <v>45811.53830461806</v>
       </c>
       <c r="AW195">
-        <v>152.713565</v>
+        <v>152.75522</v>
       </c>
     </row>
     <row r="196" ht="18" customHeight="1">
@@ -31417,7 +31417,7 @@
         <v>45825.66128076389</v>
       </c>
       <c r="AW196">
-        <v>138.59059</v>
+        <v>138.632245</v>
       </c>
     </row>
     <row r="197" ht="18" customHeight="1">
@@ -31595,7 +31595,7 @@
         <v>45813.67869909722</v>
       </c>
       <c r="AW197">
-        <v>150.573171</v>
+        <v>150.614826</v>
       </c>
     </row>
     <row r="198" ht="18" customHeight="1">
@@ -31773,7 +31773,7 @@
         <v>45821.62512202546</v>
       </c>
       <c r="AW198">
-        <v>142.626748</v>
+        <v>142.668403</v>
       </c>
     </row>
     <row r="199" ht="18" customHeight="1">
@@ -31954,7 +31954,7 @@
         <v>45859.68545269676</v>
       </c>
       <c r="AW199">
-        <v>104.566412</v>
+        <v>104.608067</v>
       </c>
     </row>
     <row r="200" ht="18" customHeight="1">
@@ -32132,7 +32132,7 @@
         <v>45859.70342961806</v>
       </c>
       <c r="AW200">
-        <v>104.548438</v>
+        <v>104.590093</v>
       </c>
     </row>
     <row r="201" ht="18" customHeight="1">
@@ -32233,7 +32233,7 @@
         <v>45937.55079028935</v>
       </c>
       <c r="AK201">
-        <v>26.701076</v>
+        <v>26.742731</v>
       </c>
     </row>
     <row r="202" ht="18" customHeight="1">
@@ -32414,7 +32414,7 @@
         <v>45954.36042099537</v>
       </c>
       <c r="AW202">
-        <v>9.891446999999999</v>
+        <v>9.933102</v>
       </c>
     </row>
     <row r="203" ht="18" customHeight="1">
@@ -32592,7 +32592,7 @@
         <v>45812.58297493056</v>
       </c>
       <c r="AW203">
-        <v>151.668889</v>
+        <v>151.710544</v>
       </c>
     </row>
     <row r="204" ht="18" customHeight="1">
@@ -32770,7 +32770,7 @@
         <v>45821.68405166667</v>
       </c>
       <c r="AW204">
-        <v>142.567813</v>
+        <v>142.609468</v>
       </c>
     </row>
     <row r="205" ht="18" customHeight="1">
@@ -32948,7 +32948,7 @@
         <v>45812.58710694444</v>
       </c>
       <c r="AW205">
-        <v>151.664757</v>
+        <v>151.706412</v>
       </c>
     </row>
     <row r="206" ht="18" customHeight="1">
@@ -33129,7 +33129,7 @@
         <v>45911.63280706019</v>
       </c>
       <c r="AW206">
-        <v>52.619063</v>
+        <v>52.660718</v>
       </c>
     </row>
     <row r="207" ht="18" customHeight="1">
@@ -33233,7 +33233,7 @@
         <v>45926.59928287037</v>
       </c>
       <c r="AK207">
-        <v>37.652581</v>
+        <v>37.694236</v>
       </c>
     </row>
     <row r="208" ht="18" customHeight="1">
@@ -33334,7 +33334,7 @@
         <v>45959.60033943287</v>
       </c>
       <c r="AK208">
-        <v>4.651528</v>
+        <v>4.693183</v>
       </c>
     </row>
     <row r="209" ht="18" customHeight="1">
@@ -33435,7 +33435,7 @@
         <v>45959.60035424768</v>
       </c>
       <c r="AK209">
-        <v>4.651516</v>
+        <v>4.693171</v>
       </c>
     </row>
     <row r="210" ht="18" customHeight="1">
@@ -33536,7 +33536,7 @@
         <v>45959.60025109954</v>
       </c>
       <c r="AK210">
-        <v>4.65162</v>
+        <v>4.693275</v>
       </c>
     </row>
     <row r="211" ht="18" customHeight="1">
@@ -33675,7 +33675,7 @@
         <v>45954.648709375</v>
       </c>
       <c r="AQ211">
-        <v>9.603160000000001</v>
+        <v>9.644814999999999</v>
       </c>
     </row>
     <row r="212" ht="18" customHeight="1">
@@ -33856,7 +33856,7 @@
         <v>45820.33415019676</v>
       </c>
       <c r="AW212">
-        <v>111.638993</v>
+        <v>111.680648</v>
       </c>
     </row>
     <row r="213" ht="18" customHeight="1">
@@ -34037,7 +34037,7 @@
         <v>45904.37834540509</v>
       </c>
       <c r="AW213">
-        <v>59.873519</v>
+        <v>59.915174</v>
       </c>
     </row>
     <row r="214" ht="18" customHeight="1">
@@ -34215,7 +34215,7 @@
         <v>45835.37156861111</v>
       </c>
       <c r="AW214">
-        <v>128.880301</v>
+        <v>128.921956</v>
       </c>
     </row>
     <row r="215" ht="18" customHeight="1">
@@ -34396,7 +34396,7 @@
         <v>45895.60195914352</v>
       </c>
       <c r="AW215">
-        <v>68.649907</v>
+        <v>68.691563</v>
       </c>
     </row>
     <row r="216" ht="18" customHeight="1">
@@ -34580,7 +34580,7 @@
         <v>45903.36175993056</v>
       </c>
       <c r="AW216">
-        <v>60.890104</v>
+        <v>60.931759</v>
       </c>
     </row>
     <row r="217" ht="18" customHeight="1">
@@ -34761,7 +34761,7 @@
         <v>45923.31386627315</v>
       </c>
       <c r="AW217">
-        <v>40.937998</v>
+        <v>40.979653</v>
       </c>
     </row>
     <row r="218" ht="18" customHeight="1">
@@ -34942,7 +34942,7 @@
         <v>45860.39721776621</v>
       </c>
       <c r="AW218">
-        <v>103.854653</v>
+        <v>103.896308</v>
       </c>
     </row>
     <row r="219" ht="18" customHeight="1">
@@ -35043,7 +35043,7 @@
         <v>45937.5506899537</v>
       </c>
       <c r="AK219">
-        <v>26.701181</v>
+        <v>26.742836</v>
       </c>
     </row>
     <row r="220" ht="18" customHeight="1">
@@ -35224,7 +35224,7 @@
         <v>45904.51875018519</v>
       </c>
       <c r="AW220">
-        <v>59.733113</v>
+        <v>59.774769</v>
       </c>
     </row>
     <row r="221" ht="18" customHeight="1">
@@ -35325,7 +35325,7 @@
         <v>45959.60020250001</v>
       </c>
       <c r="AK221">
-        <v>4.651667</v>
+        <v>4.693322</v>
       </c>
     </row>
     <row r="222" ht="18" customHeight="1">
@@ -35462,7 +35462,7 @@
         <v>45947.64590605324</v>
       </c>
       <c r="AQ222">
-        <v>16.605961</v>
+        <v>16.647616</v>
       </c>
     </row>
     <row r="223" ht="18" customHeight="1">
@@ -35643,7 +35643,7 @@
         <v>45820.33046670139</v>
       </c>
       <c r="AW223">
-        <v>93.88064799999999</v>
+        <v>93.922303</v>
       </c>
     </row>
     <row r="224" ht="18" customHeight="1">
@@ -35816,7 +35816,7 @@
         <v>45824.69872459491</v>
       </c>
       <c r="AW224">
-        <v>139.553148</v>
+        <v>139.594803</v>
       </c>
     </row>
     <row r="225" ht="18" customHeight="1">
@@ -35994,7 +35994,7 @@
         <v>45859.70464324074</v>
       </c>
       <c r="AW225">
-        <v>104.547222</v>
+        <v>104.588877</v>
       </c>
     </row>
     <row r="226" ht="18" customHeight="1">
@@ -36178,7 +36178,7 @@
         <v>45895.67057834491</v>
       </c>
       <c r="AW226">
-        <v>68.58129599999999</v>
+        <v>68.622951</v>
       </c>
     </row>
     <row r="227" ht="18" customHeight="1">
@@ -36359,7 +36359,7 @@
         <v>45952.41598819445</v>
       </c>
       <c r="AW227">
-        <v>11.83588</v>
+        <v>11.877535</v>
       </c>
     </row>
     <row r="228" ht="18" customHeight="1">
@@ -36543,7 +36543,7 @@
         <v>45923.57573010417</v>
       </c>
       <c r="AW228">
-        <v>40.640764</v>
+        <v>40.682419</v>
       </c>
     </row>
     <row r="229" ht="18" customHeight="1">
@@ -36724,7 +36724,7 @@
         <v>45929.33121140047</v>
       </c>
       <c r="AW229">
-        <v>34.92066</v>
+        <v>34.962315</v>
       </c>
     </row>
     <row r="230" ht="18" customHeight="1">
@@ -36825,7 +36825,7 @@
         <v>45936.75043002314</v>
       </c>
       <c r="AK230">
-        <v>27.501435</v>
+        <v>27.54309</v>
       </c>
     </row>
     <row r="231" ht="18" customHeight="1">
@@ -36926,7 +36926,7 @@
         <v>45959.60040009259</v>
       </c>
       <c r="AK231">
-        <v>4.65147</v>
+        <v>4.693125</v>
       </c>
     </row>
     <row r="232" ht="18" customHeight="1">
@@ -37107,7 +37107,7 @@
         <v>45888.4437121875</v>
       </c>
       <c r="AW232">
-        <v>75.80816</v>
+        <v>75.84981500000001</v>
       </c>
     </row>
     <row r="233" ht="18" customHeight="1">
@@ -37285,7 +37285,7 @@
         <v>45859.70424362268</v>
       </c>
       <c r="AW233">
-        <v>104.547627</v>
+        <v>104.589282</v>
       </c>
     </row>
     <row r="234" ht="18" customHeight="1">
@@ -37386,7 +37386,7 @@
         <v>45959.60032380787</v>
       </c>
       <c r="AK234">
-        <v>4.651551</v>
+        <v>4.693206</v>
       </c>
     </row>
     <row r="235" ht="18" customHeight="1">
@@ -37567,7 +37567,7 @@
         <v>45839.55104972223</v>
       </c>
       <c r="AW235">
-        <v>124.700822</v>
+        <v>124.742477</v>
       </c>
     </row>
     <row r="236" ht="18" customHeight="1">
@@ -37668,7 +37668,7 @@
         <v>45959.60731885416</v>
       </c>
       <c r="AK236">
-        <v>4.644549</v>
+        <v>4.686204</v>
       </c>
     </row>
     <row r="237" ht="18" customHeight="1">
@@ -37769,7 +37769,7 @@
         <v>45959.69880263889</v>
       </c>
       <c r="AK237">
-        <v>4.553067</v>
+        <v>4.594722</v>
       </c>
     </row>
     <row r="238" ht="18" customHeight="1">
@@ -37870,7 +37870,7 @@
         <v>45959.60043991898</v>
       </c>
       <c r="AK238">
-        <v>4.651424</v>
+        <v>4.693079</v>
       </c>
     </row>
     <row r="239" ht="18" customHeight="1">
@@ -38051,7 +38051,7 @@
         <v>45860.43664048611</v>
       </c>
       <c r="AW239">
-        <v>103.815231</v>
+        <v>103.856887</v>
       </c>
     </row>
     <row r="240" ht="18" customHeight="1">
@@ -38232,7 +38232,7 @@
         <v>45929.3236115625</v>
       </c>
       <c r="AW240">
-        <v>34.928252</v>
+        <v>34.969907</v>
       </c>
     </row>
     <row r="241" ht="18" customHeight="1">
@@ -38410,7 +38410,7 @@
         <v>45929.32146375</v>
       </c>
       <c r="AW241">
-        <v>34.930405</v>
+        <v>34.97206</v>
       </c>
     </row>
     <row r="242" ht="18" customHeight="1">
@@ -38588,7 +38588,7 @@
         <v>45954.73906835648</v>
       </c>
       <c r="AW242">
-        <v>9.512801</v>
+        <v>9.554456</v>
       </c>
     </row>
     <row r="243" ht="18" customHeight="1">
@@ -38689,7 +38689,7 @@
         <v>45959.60036923611</v>
       </c>
       <c r="AK243">
-        <v>4.651505</v>
+        <v>4.69316</v>
       </c>
     </row>
     <row r="244" ht="18" customHeight="1">
@@ -38865,7 +38865,7 @@
         <v>45862.4923733912</v>
       </c>
       <c r="AW244">
-        <v>101.759491</v>
+        <v>101.801146</v>
       </c>
     </row>
     <row r="245" ht="18" customHeight="1">
@@ -39043,7 +39043,7 @@
         <v>45938.33289437499</v>
       </c>
       <c r="AW245">
-        <v>25.91897</v>
+        <v>25.960625</v>
       </c>
     </row>
     <row r="246" ht="18" customHeight="1">
@@ -39227,7 +39227,7 @@
         <v>45946.65466756944</v>
       </c>
       <c r="AW246">
-        <v>11.691192</v>
+        <v>11.732847</v>
       </c>
     </row>
     <row r="247" ht="18" customHeight="1">
@@ -39408,7 +39408,7 @@
         <v>45831.5739419676</v>
       </c>
       <c r="AW247">
-        <v>132.677928</v>
+        <v>132.719583</v>
       </c>
     </row>
     <row r="248" ht="18" customHeight="1">
@@ -39586,7 +39586,7 @@
         <v>45821.62585732639</v>
       </c>
       <c r="AW248">
-        <v>142.626007</v>
+        <v>142.667662</v>
       </c>
     </row>
     <row r="249" ht="18" customHeight="1">
@@ -39767,7 +39767,7 @@
         <v>45842.71009863426</v>
       </c>
       <c r="AW249">
-        <v>121.541771</v>
+        <v>121.583426</v>
       </c>
     </row>
     <row r="250" ht="18" customHeight="1">
@@ -39871,7 +39871,7 @@
         <v>45908.53445387732</v>
       </c>
       <c r="AK250">
-        <v>55.717419</v>
+        <v>55.759074</v>
       </c>
     </row>
     <row r="251" ht="18" customHeight="1">
@@ -40049,7 +40049,7 @@
         <v>45952.55986858797</v>
       </c>
       <c r="AW251">
-        <v>11.692002</v>
+        <v>11.733657</v>
       </c>
     </row>
     <row r="252" ht="18" customHeight="1">
@@ -40191,7 +40191,7 @@
         <v>45961.71511825232</v>
       </c>
       <c r="AQ252">
-        <v>2.536748</v>
+        <v>2.578403</v>
       </c>
     </row>
     <row r="253" ht="18" customHeight="1">
@@ -40372,7 +40372,7 @@
         <v>45842.7095575463</v>
       </c>
       <c r="AW253">
-        <v>121.542315</v>
+        <v>121.58397</v>
       </c>
     </row>
     <row r="254" ht="18" customHeight="1">
@@ -40550,7 +40550,7 @@
         <v>45923.31946878473</v>
       </c>
       <c r="AW254">
-        <v>40.932396</v>
+        <v>40.974051</v>
       </c>
     </row>
     <row r="255" ht="18" customHeight="1">
@@ -40690,7 +40690,7 @@
         <v>45953.71844415509</v>
       </c>
       <c r="AQ255">
-        <v>10.602269</v>
+        <v>10.643924</v>
       </c>
     </row>
     <row r="256" ht="18" customHeight="1">
@@ -40871,7 +40871,7 @@
         <v>45832.68075126158</v>
       </c>
       <c r="AW256">
-        <v>131.571123</v>
+        <v>131.612778</v>
       </c>
     </row>
     <row r="257" ht="18" customHeight="1">
@@ -41052,7 +41052,7 @@
         <v>45846.4887596412</v>
       </c>
       <c r="AW257">
-        <v>117.763113</v>
+        <v>117.804769</v>
       </c>
     </row>
     <row r="258" ht="18" customHeight="1">
@@ -41233,7 +41233,7 @@
         <v>45917.46522068288</v>
       </c>
       <c r="AW258">
-        <v>46.786644</v>
+        <v>46.828299</v>
       </c>
     </row>
     <row r="259" ht="18" customHeight="1">
@@ -41334,7 +41334,7 @@
         <v>45959.60016287037</v>
       </c>
       <c r="AK259">
-        <v>4.651701</v>
+        <v>4.693356</v>
       </c>
     </row>
     <row r="260" ht="18" customHeight="1">
@@ -41447,7 +41447,7 @@
         <v>45958.37969225695</v>
       </c>
       <c r="AN260">
-        <v>5.872176</v>
+        <v>5.913831</v>
       </c>
     </row>
     <row r="261" ht="18" customHeight="1">
@@ -41608,7 +41608,7 @@
         <v>45960.48726086806</v>
       </c>
       <c r="AT261">
-        <v>3.764606</v>
+        <v>3.806262</v>
       </c>
     </row>
     <row r="262" ht="18" customHeight="1">
@@ -41747,7 +41747,7 @@
         <v>45954.64880266204</v>
       </c>
       <c r="AQ262">
-        <v>9.603066999999999</v>
+        <v>9.644722</v>
       </c>
     </row>
     <row r="263" ht="18" customHeight="1">
@@ -41931,7 +41931,7 @@
         <v>45924.33433900463</v>
       </c>
       <c r="AW263">
-        <v>26.922396</v>
+        <v>26.964051</v>
       </c>
     </row>
     <row r="264" ht="18" customHeight="1">
@@ -42032,7 +42032,7 @@
         <v>45959.60015383102</v>
       </c>
       <c r="AK264">
-        <v>4.651713</v>
+        <v>4.693368</v>
       </c>
     </row>
     <row r="265" ht="18" customHeight="1">
@@ -42210,7 +42210,7 @@
         <v>45845.32248731481</v>
       </c>
       <c r="AW265">
-        <v>118.929387</v>
+        <v>118.971042</v>
       </c>
     </row>
     <row r="266" ht="18" customHeight="1">
@@ -42388,7 +42388,7 @@
         <v>45833.56582039352</v>
       </c>
       <c r="AW266">
-        <v>130.686053</v>
+        <v>130.727708</v>
       </c>
     </row>
     <row r="267" ht="18" customHeight="1">
@@ -42569,7 +42569,7 @@
         <v>45890.64208997686</v>
       </c>
       <c r="AW267">
-        <v>73.60978</v>
+        <v>73.65143500000001</v>
       </c>
     </row>
     <row r="268" ht="18" customHeight="1">
@@ -42750,7 +42750,7 @@
         <v>45846.36008232638</v>
       </c>
       <c r="AW268">
-        <v>117.891782</v>
+        <v>117.933438</v>
       </c>
     </row>
     <row r="269" ht="18" customHeight="1">
@@ -42928,7 +42928,7 @@
         <v>45870.37016001157</v>
       </c>
       <c r="AW269">
-        <v>93.881713</v>
+        <v>93.923368</v>
       </c>
     </row>
     <row r="270" ht="18" customHeight="1">
@@ -43112,7 +43112,7 @@
         <v>45944.44625667824</v>
       </c>
       <c r="AW270">
-        <v>14.937199</v>
+        <v>14.978854</v>
       </c>
     </row>
     <row r="271" ht="18" customHeight="1">
@@ -43213,7 +43213,7 @@
         <v>45937.55078203704</v>
       </c>
       <c r="AK271">
-        <v>26.701088</v>
+        <v>26.742743</v>
       </c>
     </row>
     <row r="272" ht="18" customHeight="1">
@@ -43350,7 +43350,7 @@
         <v>45953.71873744213</v>
       </c>
       <c r="AQ272">
-        <v>10.613866</v>
+        <v>10.655521</v>
       </c>
     </row>
     <row r="273" ht="18" customHeight="1">
@@ -43528,7 +43528,7 @@
         <v>45832.3608832176</v>
       </c>
       <c r="AW273">
-        <v>131.890984</v>
+        <v>131.932639</v>
       </c>
     </row>
     <row r="274" ht="18" customHeight="1">
@@ -43709,7 +43709,7 @@
         <v>45887.75298732638</v>
       </c>
       <c r="AW274">
-        <v>76.49887699999999</v>
+        <v>76.540532</v>
       </c>
     </row>
     <row r="275" ht="18" customHeight="1">
@@ -43887,7 +43887,7 @@
         <v>45826.76998138889</v>
       </c>
       <c r="AW275">
-        <v>137.481887</v>
+        <v>137.523542</v>
       </c>
     </row>
     <row r="276" ht="18" customHeight="1">
@@ -44068,7 +44068,7 @@
         <v>45904.37713482638</v>
       </c>
       <c r="AW276">
-        <v>59.874734</v>
+        <v>59.916389</v>
       </c>
     </row>
     <row r="277" ht="18" customHeight="1">
@@ -44246,7 +44246,7 @@
         <v>45859.70231407408</v>
       </c>
       <c r="AW277">
-        <v>104.54956</v>
+        <v>104.591215</v>
       </c>
     </row>
     <row r="278" ht="18" customHeight="1">
@@ -44350,7 +44350,7 @@
         <v>45908.5344964699</v>
       </c>
       <c r="AK278">
-        <v>55.717373</v>
+        <v>55.759028</v>
       </c>
     </row>
     <row r="279" ht="18" customHeight="1">
@@ -44539,7 +44539,7 @@
         <v>45835.37110386574</v>
       </c>
       <c r="AW279">
-        <v>128.880764</v>
+        <v>128.922419</v>
       </c>
     </row>
     <row r="280" ht="18" customHeight="1">
@@ -44720,7 +44720,7 @@
         <v>45904.38426976852</v>
       </c>
       <c r="AW280">
-        <v>59.867604</v>
+        <v>59.909259</v>
       </c>
     </row>
     <row r="281" ht="18" customHeight="1">
@@ -44898,7 +44898,7 @@
         <v>45929.57279483796</v>
       </c>
       <c r="AW281">
-        <v>34.679074</v>
+        <v>34.720729</v>
       </c>
     </row>
     <row r="282" ht="18" customHeight="1">
@@ -44999,7 +44999,7 @@
         <v>45959.6001878125</v>
       </c>
       <c r="AK282">
-        <v>4.651678</v>
+        <v>4.693333</v>
       </c>
     </row>
     <row r="283" ht="18" customHeight="1">
@@ -45177,7 +45177,7 @@
         <v>45820.33137869213</v>
       </c>
       <c r="AW283">
-        <v>143.920486</v>
+        <v>143.962141</v>
       </c>
     </row>
     <row r="284" ht="18" customHeight="1">
@@ -45363,7 +45363,7 @@
         <v>45894.61132443287</v>
       </c>
       <c r="AW284">
-        <v>69.64054400000001</v>
+        <v>69.682199</v>
       </c>
     </row>
     <row r="285" ht="18" customHeight="1">
@@ -45544,7 +45544,7 @@
         <v>45930.65916848379</v>
       </c>
       <c r="AW285">
-        <v>33.592697</v>
+        <v>33.634352</v>
       </c>
     </row>
     <row r="286" ht="18" customHeight="1">
@@ -45648,7 +45648,7 @@
         <v>45926.59934261574</v>
       </c>
       <c r="AK286">
-        <v>37.652523</v>
+        <v>37.694178</v>
       </c>
     </row>
     <row r="287" ht="18" customHeight="1">
@@ -45749,7 +45749,7 @@
         <v>45959.60011650463</v>
       </c>
       <c r="AK287">
-        <v>4.651748</v>
+        <v>4.693403</v>
       </c>
     </row>
     <row r="288" ht="18" customHeight="1">
@@ -45850,7 +45850,7 @@
         <v>45959.60043074074</v>
       </c>
       <c r="AK288">
-        <v>4.651435</v>
+        <v>4.69309</v>
       </c>
     </row>
     <row r="289" ht="18" customHeight="1">
@@ -46031,7 +46031,7 @@
         <v>45930.65883226852</v>
       </c>
       <c r="AW289">
-        <v>33.593032</v>
+        <v>33.634688</v>
       </c>
     </row>
     <row r="290" ht="18" customHeight="1">
@@ -46212,7 +46212,7 @@
         <v>45930.6606075926</v>
       </c>
       <c r="AW290">
-        <v>33.591262</v>
+        <v>33.632917</v>
       </c>
     </row>
     <row r="291" ht="18" customHeight="1">
@@ -46313,7 +46313,7 @@
         <v>45936.75043699074</v>
       </c>
       <c r="AK291">
-        <v>27.501435</v>
+        <v>27.54309</v>
       </c>
     </row>
     <row r="292" ht="18" customHeight="1">
@@ -46491,7 +46491,7 @@
         <v>45826.76959586806</v>
       </c>
       <c r="AW292">
-        <v>137.482269</v>
+        <v>137.523924</v>
       </c>
     </row>
     <row r="293" ht="18" customHeight="1">
@@ -46672,7 +46672,7 @@
         <v>45873.70791493055</v>
       </c>
       <c r="AW293">
-        <v>90.543958</v>
+        <v>90.585613</v>
       </c>
     </row>
     <row r="294" ht="18" customHeight="1">
@@ -46853,7 +46853,7 @@
         <v>45954.62754329861</v>
       </c>
       <c r="AW294">
-        <v>9.624328999999999</v>
+        <v>9.665984</v>
       </c>
     </row>
     <row r="295" ht="18" customHeight="1">
@@ -47034,7 +47034,7 @@
         <v>45873.70610516204</v>
       </c>
       <c r="AW295">
-        <v>90.54674799999999</v>
+        <v>90.588403</v>
       </c>
     </row>
     <row r="296" ht="18" customHeight="1">
@@ -47215,7 +47215,7 @@
         <v>45840.40468760417</v>
       </c>
       <c r="AW296">
-        <v>103.851991</v>
+        <v>103.893646</v>
       </c>
     </row>
     <row r="297" ht="18" customHeight="1">
@@ -47393,7 +47393,7 @@
         <v>45817.43653768519</v>
       </c>
       <c r="AW297">
-        <v>146.815336</v>
+        <v>146.856991</v>
       </c>
     </row>
     <row r="298" ht="18" customHeight="1">
@@ -47574,7 +47574,7 @@
         <v>45923.32032945602</v>
       </c>
       <c r="AW298">
-        <v>40.931539</v>
+        <v>40.973194</v>
       </c>
     </row>
     <row r="299" ht="18" customHeight="1">
@@ -47752,7 +47752,7 @@
         <v>45959.61025383102</v>
       </c>
       <c r="AW299">
-        <v>4.64162</v>
+        <v>4.683275</v>
       </c>
     </row>
     <row r="300" ht="18" customHeight="1">
@@ -47865,7 +47865,7 @@
         <v>45945.73041342592</v>
       </c>
       <c r="AN300">
-        <v>18.521458</v>
+        <v>18.563113</v>
       </c>
     </row>
     <row r="301" ht="18" customHeight="1">
@@ -48046,7 +48046,7 @@
         <v>45883.60346527777</v>
       </c>
       <c r="AW301">
-        <v>80.648403</v>
+        <v>80.69005799999999</v>
       </c>
     </row>
     <row r="302" ht="18" customHeight="1">
@@ -48227,7 +48227,7 @@
         <v>45838.66248615741</v>
       </c>
       <c r="AW302">
-        <v>125.589387</v>
+        <v>125.631042</v>
       </c>
     </row>
     <row r="303" ht="18" customHeight="1">
@@ -48328,7 +48328,7 @@
         <v>45959.60021726852</v>
       </c>
       <c r="AK303">
-        <v>4.651655</v>
+        <v>4.69331</v>
       </c>
     </row>
     <row r="304" ht="18" customHeight="1">
@@ -48429,7 +48429,7 @@
         <v>45959.60025849537</v>
       </c>
       <c r="AK304">
-        <v>4.651609</v>
+        <v>4.693264</v>
       </c>
     </row>
     <row r="305" ht="18" customHeight="1">
@@ -48607,7 +48607,7 @@
         <v>45859.70298075231</v>
       </c>
       <c r="AW305">
-        <v>104.548889</v>
+        <v>104.590544</v>
       </c>
     </row>
     <row r="306" ht="18" customHeight="1">
@@ -48785,7 +48785,7 @@
         <v>45890.69609947917</v>
       </c>
       <c r="AW306">
-        <v>73.555775</v>
+        <v>73.597431</v>
       </c>
     </row>
     <row r="307" ht="18" customHeight="1">
@@ -48969,7 +48969,7 @@
         <v>45944.68359482639</v>
       </c>
       <c r="AW307">
-        <v>19.566493</v>
+        <v>19.608148</v>
       </c>
     </row>
     <row r="308" ht="18" customHeight="1">
@@ -49079,7 +49079,7 @@
         <v>45947.74728230324</v>
       </c>
       <c r="AN308">
-        <v>16.504583</v>
+        <v>16.546238</v>
       </c>
     </row>
     <row r="309" ht="18" customHeight="1">
@@ -49240,7 +49240,7 @@
         <v>45960.48738048611</v>
       </c>
       <c r="AT309">
-        <v>3.764491</v>
+        <v>3.806146</v>
       </c>
     </row>
     <row r="310" ht="18" customHeight="1">
@@ -49418,7 +49418,7 @@
         <v>45880.67850293982</v>
       </c>
       <c r="AW310">
-        <v>83.573368</v>
+        <v>83.61502299999999</v>
       </c>
     </row>
     <row r="311" ht="18" customHeight="1">
@@ -49519,7 +49519,7 @@
         <v>45959.60019512731</v>
       </c>
       <c r="AK311">
-        <v>4.651678</v>
+        <v>4.693333</v>
       </c>
     </row>
     <row r="312" ht="18" customHeight="1">
@@ -49700,7 +49700,7 @@
         <v>45888.44706435185</v>
       </c>
       <c r="AW312">
-        <v>75.80480300000001</v>
+        <v>75.846458</v>
       </c>
     </row>
     <row r="313" ht="18" customHeight="1">
@@ -49876,7 +49876,7 @@
         <v>45954.62802541666</v>
       </c>
       <c r="AW313">
-        <v>9.623843000000001</v>
+        <v>9.665497999999999</v>
       </c>
     </row>
     <row r="314" ht="18" customHeight="1">
@@ -50054,7 +50054,7 @@
         <v>45812.5781485301</v>
       </c>
       <c r="AW314">
-        <v>151.673715</v>
+        <v>151.71537</v>
       </c>
     </row>
     <row r="315" ht="18" customHeight="1">
@@ -50235,7 +50235,7 @@
         <v>45902.37917880787</v>
       </c>
       <c r="AW315">
-        <v>61.872685</v>
+        <v>61.91434</v>
       </c>
     </row>
     <row r="316" ht="18" customHeight="1">
@@ -50416,7 +50416,7 @@
         <v>45923.31296491898</v>
       </c>
       <c r="AW316">
-        <v>40.9389</v>
+        <v>40.980556</v>
       </c>
     </row>
     <row r="317" ht="18" customHeight="1">
@@ -50520,7 +50520,7 @@
         <v>45926.59932865741</v>
       </c>
       <c r="AK317">
-        <v>37.652546</v>
+        <v>37.694201</v>
       </c>
     </row>
     <row r="318" ht="18" customHeight="1">
@@ -50701,7 +50701,7 @@
         <v>45855.33980681713</v>
       </c>
       <c r="AW318">
-        <v>108.91206</v>
+        <v>108.953715</v>
       </c>
     </row>
     <row r="319" ht="18" customHeight="1">
@@ -50802,7 +50802,7 @@
         <v>45959.60026587963</v>
       </c>
       <c r="AK319">
-        <v>4.651609</v>
+        <v>4.693264</v>
       </c>
     </row>
     <row r="320" ht="18" customHeight="1">
@@ -50903,7 +50903,7 @@
         <v>45959.60021008101</v>
       </c>
       <c r="AK320">
-        <v>4.651655</v>
+        <v>4.69331</v>
       </c>
     </row>
     <row r="321" ht="18" customHeight="1">
@@ -51004,7 +51004,7 @@
         <v>45959.60017260416</v>
       </c>
       <c r="AK321">
-        <v>4.651701</v>
+        <v>4.693356</v>
       </c>
     </row>
     <row r="322" ht="18" customHeight="1">
@@ -51182,7 +51182,7 @@
         <v>45898.61942834491</v>
       </c>
       <c r="AW322">
-        <v>65.632442</v>
+        <v>65.674097</v>
       </c>
     </row>
     <row r="323" ht="18" customHeight="1">
@@ -51363,7 +51363,7 @@
         <v>45919.68091108797</v>
       </c>
       <c r="AW323">
-        <v>44.570961</v>
+        <v>44.612616</v>
       </c>
     </row>
     <row r="324" ht="18" customHeight="1">
@@ -51541,7 +51541,7 @@
         <v>45954.62691407408</v>
       </c>
       <c r="AW324">
-        <v>9.624954000000001</v>
+        <v>9.666608999999999</v>
       </c>
     </row>
     <row r="325" ht="18" customHeight="1">
@@ -51651,7 +51651,7 @@
         <v>45947.74624858797</v>
       </c>
       <c r="AN325">
-        <v>16.505625</v>
+        <v>16.54728</v>
       </c>
     </row>
     <row r="326" ht="18" customHeight="1">
@@ -51832,7 +51832,7 @@
         <v>45846.35986268519</v>
       </c>
       <c r="AW326">
-        <v>117.892002</v>
+        <v>117.933657</v>
       </c>
     </row>
     <row r="327" ht="18" customHeight="1">
@@ -52013,7 +52013,7 @@
         <v>45917.46567336806</v>
       </c>
       <c r="AW327">
-        <v>46.786192</v>
+        <v>46.827847</v>
       </c>
     </row>
     <row r="328" ht="18" customHeight="1">
@@ -52194,7 +52194,7 @@
         <v>45929.33197420138</v>
       </c>
       <c r="AW328">
-        <v>34.919896</v>
+        <v>34.961551</v>
       </c>
     </row>
     <row r="329" ht="18" customHeight="1">
@@ -52375,7 +52375,7 @@
         <v>45915.4691385301</v>
       </c>
       <c r="AW329">
-        <v>40.992407</v>
+        <v>41.034063</v>
       </c>
     </row>
     <row r="330" ht="18" customHeight="1">
@@ -52476,7 +52476,7 @@
         <v>45936.75049591436</v>
       </c>
       <c r="AK330">
-        <v>27.501377</v>
+        <v>27.543032</v>
       </c>
     </row>
     <row r="331" ht="18" customHeight="1">
@@ -52577,7 +52577,7 @@
         <v>45959.60014600695</v>
       </c>
       <c r="AK331">
-        <v>4.651725</v>
+        <v>4.69338</v>
       </c>
     </row>
     <row r="332" ht="18" customHeight="1">
@@ -52758,7 +52758,7 @@
         <v>45821.67524549768</v>
       </c>
       <c r="AW332">
-        <v>142.57662</v>
+        <v>142.618275</v>
       </c>
     </row>
     <row r="333" ht="18" customHeight="1">
@@ -52936,7 +52936,7 @@
         <v>45820.3330696875</v>
       </c>
       <c r="AW333">
-        <v>143.918796</v>
+        <v>143.960451</v>
       </c>
     </row>
     <row r="334" ht="18" customHeight="1">
@@ -53037,7 +53037,7 @@
         <v>45951.64880866898</v>
       </c>
       <c r="AK334">
-        <v>12.603056</v>
+        <v>12.644711</v>
       </c>
     </row>
     <row r="335" ht="18" customHeight="1">
@@ -53138,7 +53138,7 @@
         <v>45959.60024362268</v>
       </c>
       <c r="AK335">
-        <v>4.65162</v>
+        <v>4.693275</v>
       </c>
     </row>
     <row r="336" ht="18" customHeight="1">
@@ -53316,7 +53316,7 @@
         <v>45813.68440848379</v>
       </c>
       <c r="AW336">
-        <v>150.567465</v>
+        <v>150.60912</v>
       </c>
     </row>
     <row r="337" ht="18" customHeight="1">
@@ -53497,7 +53497,7 @@
         <v>45923.31175675926</v>
       </c>
       <c r="AW337">
-        <v>40.940116</v>
+        <v>40.981771</v>
       </c>
     </row>
     <row r="338" ht="18" customHeight="1">
@@ -53678,7 +53678,7 @@
         <v>45842.70903693287</v>
       </c>
       <c r="AW338">
-        <v>121.542836</v>
+        <v>121.584491</v>
       </c>
     </row>
     <row r="339" ht="18" customHeight="1">
@@ -53859,7 +53859,7 @@
         <v>45952.41448010417</v>
       </c>
       <c r="AW339">
-        <v>11.837384</v>
+        <v>11.879039</v>
       </c>
     </row>
     <row r="340" ht="18" customHeight="1">
@@ -54040,7 +54040,7 @@
         <v>45954.37944618055</v>
       </c>
       <c r="AW340">
-        <v>9.872419000000001</v>
+        <v>9.914073999999999</v>
       </c>
     </row>
     <row r="341" ht="18" customHeight="1">
@@ -54218,7 +54218,7 @@
         <v>45826.77024422454</v>
       </c>
       <c r="AW341">
-        <v>137.48162</v>
+        <v>137.523275</v>
       </c>
     </row>
     <row r="342" ht="18" customHeight="1">
@@ -54399,7 +54399,7 @@
         <v>45855.34249084491</v>
       </c>
       <c r="AW342">
-        <v>108.909375</v>
+        <v>108.95103</v>
       </c>
     </row>
     <row r="343" ht="18" customHeight="1">
@@ -54577,7 +54577,7 @@
         <v>45936.74229829861</v>
       </c>
       <c r="AW343">
-        <v>27.509572</v>
+        <v>27.551227</v>
       </c>
     </row>
     <row r="344" ht="18" customHeight="1">
@@ -54755,7 +54755,7 @@
         <v>45852.54993511573</v>
       </c>
       <c r="AW344">
-        <v>111.701933</v>
+        <v>111.743588</v>
       </c>
     </row>
     <row r="345" ht="18" customHeight="1">
@@ -54936,7 +54936,7 @@
         <v>45904.38291060185</v>
       </c>
       <c r="AW345">
-        <v>59.868958</v>
+        <v>59.910613</v>
       </c>
     </row>
     <row r="346" ht="18" customHeight="1">
@@ -55114,7 +55114,7 @@
         <v>45810.36123126157</v>
       </c>
       <c r="AW346">
-        <v>146.707373</v>
+        <v>146.749028</v>
       </c>
     </row>
     <row r="347" ht="18" customHeight="1">
@@ -55292,7 +55292,7 @@
         <v>45821.63864346065</v>
       </c>
       <c r="AW347">
-        <v>142.613229</v>
+        <v>142.654884</v>
       </c>
     </row>
     <row r="348" ht="18" customHeight="1">
@@ -55405,7 +55405,7 @@
         <v>45952.60817993055</v>
       </c>
       <c r="AN348">
-        <v>11.643692</v>
+        <v>11.685347</v>
       </c>
     </row>
     <row r="349" ht="18" customHeight="1">
@@ -55583,7 +55583,7 @@
         <v>45820.3322787037</v>
       </c>
       <c r="AW349">
-        <v>143.919595</v>
+        <v>143.96125</v>
       </c>
     </row>
     <row r="350" ht="18" customHeight="1">
@@ -55761,7 +55761,7 @@
         <v>45842.70851819444</v>
       </c>
       <c r="AW350">
-        <v>121.543356</v>
+        <v>121.585012</v>
       </c>
     </row>
     <row r="351" ht="18" customHeight="1">
@@ -55939,7 +55939,7 @@
         <v>45812.58675498843</v>
       </c>
       <c r="AW351">
-        <v>151.665116</v>
+        <v>151.706771</v>
       </c>
     </row>
     <row r="352" ht="18" customHeight="1">
@@ -56081,7 +56081,7 @@
         <v>45953.71864649306</v>
       </c>
       <c r="AQ352">
-        <v>10.60772</v>
+        <v>10.649375</v>
       </c>
     </row>
     <row r="353" ht="18" customHeight="1">
@@ -56259,7 +56259,7 @@
         <v>45826.77171652778</v>
       </c>
       <c r="AW353">
-        <v>137.48015</v>
+        <v>137.521806</v>
       </c>
     </row>
     <row r="354" ht="18" customHeight="1">
@@ -56437,7 +56437,7 @@
         <v>45859.70584207177</v>
       </c>
       <c r="AW354">
-        <v>104.54603</v>
+        <v>104.587685</v>
       </c>
     </row>
     <row r="355" ht="18" customHeight="1">
@@ -56618,7 +56618,7 @@
         <v>45868.57320862269</v>
       </c>
       <c r="AW355">
-        <v>95.678657</v>
+        <v>95.720313</v>
       </c>
     </row>
     <row r="356" ht="18" customHeight="1">
@@ -56719,7 +56719,7 @@
         <v>45937.55069800926</v>
       </c>
       <c r="AK356">
-        <v>26.701169</v>
+        <v>26.742824</v>
       </c>
     </row>
     <row r="357" ht="18" customHeight="1">
@@ -56900,7 +56900,7 @@
         <v>45952.41516831018</v>
       </c>
       <c r="AW357">
-        <v>11.836701</v>
+        <v>11.878356</v>
       </c>
     </row>
     <row r="358" ht="18" customHeight="1">
@@ -57001,7 +57001,7 @@
         <v>45959.6002246412</v>
       </c>
       <c r="AK358">
-        <v>4.651644</v>
+        <v>4.693299</v>
       </c>
     </row>
     <row r="359" ht="18" customHeight="1">
@@ -57174,7 +57174,7 @@
         <v>45905.67968340278</v>
       </c>
       <c r="AW359">
-        <v>58.572188</v>
+        <v>58.613843</v>
       </c>
     </row>
     <row r="360" ht="18" customHeight="1">
@@ -57347,7 +57347,7 @@
         <v>45905.68014417824</v>
       </c>
       <c r="AW360">
-        <v>58.571725</v>
+        <v>58.61338</v>
       </c>
     </row>
     <row r="361" ht="18" customHeight="1">
@@ -57448,7 +57448,7 @@
         <v>45959.60010946759</v>
       </c>
       <c r="AK361">
-        <v>4.651759</v>
+        <v>4.693414</v>
       </c>
     </row>
     <row r="362" ht="18" customHeight="1">
@@ -57552,7 +57552,7 @@
         <v>45926.59936648148</v>
       </c>
       <c r="AK362">
-        <v>37.6525</v>
+        <v>37.694155</v>
       </c>
     </row>
     <row r="363" ht="18" customHeight="1">
@@ -57691,7 +57691,7 @@
         <v>45954.64856469908</v>
       </c>
       <c r="AQ363">
-        <v>9.60331</v>
+        <v>9.644964999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>